<commit_message>
modified template .sky file
</commit_message>
<xml_diff>
--- a/Example_data/Example_transition_list.xlsx
+++ b/Example_data/Example_transition_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdabke/Documents/chapter_automation/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdabke/Documents/GitHub/Chapter-Skyline-Automation/Example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F18934AF-6B6D-204E-9824-B90788E95452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3473370-9B5A-834C-A214-96BEB902D683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{8AFE52A1-B9EE-794B-9FFC-391CA2EF1745}"/>
+    <workbookView xWindow="10360" yWindow="2460" windowWidth="28040" windowHeight="17440" xr2:uid="{8AFE52A1-B9EE-794B-9FFC-391CA2EF1745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,23 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>Molecule Name</t>
   </si>
   <si>
-    <t>Molecule list</t>
-  </si>
-  <si>
-    <t>Precursor Neutral Formula</t>
-  </si>
-  <si>
-    <t>Precursor Neutral Mass</t>
-  </si>
-  <si>
-    <t>Precursor Mz</t>
-  </si>
-  <si>
     <t>Precursor Adduct</t>
   </si>
   <si>
@@ -146,20 +134,38 @@
     <t>[M18C13-H]</t>
   </si>
   <si>
-    <t>13C6-Sucrose</t>
-  </si>
-  <si>
-    <t>C12H22O11</t>
-  </si>
-  <si>
     <t>Explicit Retention Time</t>
+  </si>
+  <si>
+    <t>Molecule List Name</t>
+  </si>
+  <si>
+    <t>Molecule Formula</t>
+  </si>
+  <si>
+    <t>[M3C13+H]</t>
+  </si>
+  <si>
+    <t>[M6C13+H]</t>
+  </si>
+  <si>
+    <t>[M11C13+H]</t>
+  </si>
+  <si>
+    <t>[M10D+H]</t>
+  </si>
+  <si>
+    <t>13C3-Caffeine</t>
+  </si>
+  <si>
+    <t>C8H10N4O2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,21 +175,10 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,11 +201,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,275 +538,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ED16F9-7B13-1D44-B37C-5D96A43DF589}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E2" s="1">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3">
-        <v>92.057699999999997</v>
-      </c>
-      <c r="E2" s="2">
-        <v>91.0505</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3">
-        <v>137.1148</v>
-      </c>
-      <c r="E3" s="2">
-        <v>136.10749999999999</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3">
-        <v>171.09909999999999</v>
-      </c>
-      <c r="E4" s="2">
-        <v>170.09180000000001</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3">
-        <v>187.09399999999999</v>
-      </c>
-      <c r="E5" s="2">
-        <v>186.08680000000001</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="E18" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3">
-        <v>215.1268</v>
-      </c>
-      <c r="E6" s="2">
-        <v>214.11949999999999</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3">
-        <v>122.04</v>
-      </c>
-      <c r="E7" s="2">
-        <v>121.03279999999999</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3">
-        <v>128.05690000000001</v>
-      </c>
-      <c r="E8" s="2">
-        <v>127.0496</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3">
-        <v>141.1574</v>
-      </c>
-      <c r="E9" s="2">
-        <v>140.15010000000001</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="3">
-        <v>152.14189999999999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>151.13460000000001</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="3">
-        <v>195.03710000000001</v>
-      </c>
-      <c r="E11" s="2">
-        <v>194.02979999999999</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="3">
-        <v>302.33190000000002</v>
-      </c>
-      <c r="E12" s="2">
-        <v>301.32470000000001</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3">
-        <v>348.13630000000001</v>
-      </c>
-      <c r="E13" s="2">
-        <v>347.12909999999999</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
+      <c r="E19" s="1">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>